<commit_message>
update documentation + favicon
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
   <si>
     <t>Journal de bord du pre-TPI</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>Création du MCD et du MLD de la base de données.</t>
+  </si>
+  <si>
+    <t>Début de la création du README</t>
+  </si>
+  <si>
+    <t>Réalisation / finition du serveur de distribution de fichiers</t>
+  </si>
+  <si>
+    <t>Analyse et conception du serveur de distribution de fichiers (et un peu du serveur http)</t>
   </si>
 </sst>
 </file>
@@ -720,8 +729,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,16 +949,16 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="9">
+      <c r="A17" s="11">
         <v>43529</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="16" t="s">
+      <c r="C17" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="D17" s="23" t="s">
         <v>30</v>
       </c>
     </row>
@@ -983,7 +992,7 @@
       <c r="A20" s="12">
         <v>43532</v>
       </c>
-      <c r="B20" s="24" t="s">
+      <c r="B20" s="15" t="s">
         <v>38</v>
       </c>
       <c r="C20" s="16" t="s">
@@ -994,37 +1003,53 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="B21" s="15" t="s">
+      <c r="A21" s="10"/>
+      <c r="B21" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="17" t="s">
+      <c r="D21" s="20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="9"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="17"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>43538</v>
+      </c>
+      <c r="B22" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="22"/>
+      <c r="D22" s="23" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="9"/>
-      <c r="B23" s="15"/>
+      <c r="B23" s="15" t="s">
+        <v>20</v>
+      </c>
       <c r="C23" s="16"/>
-      <c r="D23" s="17"/>
+      <c r="D23" s="17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="9"/>
-      <c r="B24" s="15"/>
+      <c r="B24" s="15" t="s">
+        <v>38</v>
+      </c>
       <c r="C24" s="16"/>
-      <c r="D24" s="17"/>
+      <c r="D24" s="17" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="9"/>
+      <c r="A25" s="9">
+        <v>43539</v>
+      </c>
       <c r="B25" s="15"/>
       <c r="C25" s="16"/>
       <c r="D25" s="17"/>

</xml_diff>

<commit_message>
updated MCD & MLD
</commit_message>
<xml_diff>
--- a/documentation/MAITRE_JournalDeBord.xlsx
+++ b/documentation/MAITRE_JournalDeBord.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="46">
   <si>
     <t>Journal de bord du pre-TPI</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>Analyse et conception du serveur de distribution de fichiers (et un peu du serveur http)</t>
+  </si>
+  <si>
+    <t>Création du framwork de construction de la page en Javascript (gestionnaire de pages)</t>
+  </si>
+  <si>
+    <t>Création du topMenu de la page MWA</t>
   </si>
 </sst>
 </file>
@@ -730,7 +736,7 @@
   <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,19 +1052,31 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="9">
         <v>43539</v>
       </c>
-      <c r="B25" s="15"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="17"/>
+      <c r="B25" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="9"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D26" s="17" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>

</xml_diff>